<commit_message>
ESCALETA Y MAPA ACTUALIZADOS 10_07
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion07/Escaleta_CN_10_07_CO.xlsx
+++ b/fuentes/contenidos/grado10/guion07/Escaleta_CN_10_07_CO.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PLANETA 10 Y 11\CN_10_07_CO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado10\guion07\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1155,6 +1155,12 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1223,12 +1229,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="85">
@@ -1422,6 +1422,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1457,6 +1474,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1636,9 +1670,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:U120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J21" sqref="J21"/>
+      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1667,94 +1701,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="3" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="83" t="s">
+      <c r="C1" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="74" t="s">
+      <c r="D1" s="76" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="72" t="s">
+      <c r="E1" s="74" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="70" t="s">
+      <c r="F1" s="72" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="76" t="s">
+      <c r="G1" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="70" t="s">
+      <c r="H1" s="72" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="70" t="s">
+      <c r="I1" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="80" t="s">
+      <c r="J1" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="78" t="s">
+      <c r="K1" s="80" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="76" t="s">
+      <c r="L1" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="82" t="s">
+      <c r="M1" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="82"/>
-      <c r="O1" s="62" t="s">
+      <c r="N1" s="84"/>
+      <c r="O1" s="64" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="62" t="s">
+      <c r="P1" s="64" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="64" t="s">
+      <c r="Q1" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="68" t="s">
+      <c r="R1" s="70" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="64" t="s">
+      <c r="S1" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="66" t="s">
+      <c r="T1" s="68" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="64" t="s">
+      <c r="U1" s="66" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="75"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="77"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="79"/>
       <c r="M2" s="4" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="69"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="67"/>
-      <c r="U2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="71"/>
+      <c r="S2" s="67"/>
+      <c r="T2" s="69"/>
+      <c r="U2" s="67"/>
     </row>
     <row r="3" spans="1:21" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -1797,19 +1831,19 @@
       <c r="P3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="85">
+      <c r="Q3" s="62">
         <v>9</v>
       </c>
-      <c r="R3" s="85" t="s">
+      <c r="R3" s="62" t="s">
         <v>214</v>
       </c>
-      <c r="S3" s="85" t="s">
+      <c r="S3" s="62" t="s">
         <v>213</v>
       </c>
-      <c r="T3" s="86" t="s">
+      <c r="T3" s="63" t="s">
         <v>212</v>
       </c>
-      <c r="U3" s="85" t="s">
+      <c r="U3" s="62" t="s">
         <v>215</v>
       </c>
     </row>
@@ -2239,50 +2273,50 @@
       <c r="D11" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="E11" s="35" t="s">
-        <v>156</v>
-      </c>
-      <c r="F11" s="36"/>
+      <c r="E11" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="F11" s="25"/>
       <c r="G11" s="9" t="s">
-        <v>171</v>
+        <v>186</v>
       </c>
       <c r="H11" s="8">
         <v>9</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="20" t="s">
         <v>19</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="L11" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="K11" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="M11" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="N11" s="12"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13" t="s">
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="P11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="14">
-        <v>6</v>
+      <c r="Q11" s="14" t="s">
+        <v>146</v>
       </c>
       <c r="R11" s="15" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="S11" s="14" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="T11" s="16" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="U11" s="14" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2299,11 +2333,11 @@
         <v>155</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="9" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="H12" s="8">
         <v>10</v>
@@ -2312,34 +2346,36 @@
         <v>20</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>169</v>
+        <v>205</v>
       </c>
       <c r="K12" s="21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L12" s="22" t="s">
         <v>8</v>
       </c>
       <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
+      <c r="N12" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="O12" s="19"/>
       <c r="P12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="R12" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="S12" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="T12" s="28" t="s">
-        <v>168</v>
-      </c>
-      <c r="U12" s="26" t="s">
-        <v>150</v>
+      <c r="Q12" s="14">
+        <v>6</v>
+      </c>
+      <c r="R12" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="S12" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="T12" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="U12" s="14" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2360,45 +2396,45 @@
       </c>
       <c r="F13" s="25"/>
       <c r="G13" s="9" t="s">
-        <v>186</v>
+        <v>209</v>
       </c>
       <c r="H13" s="8">
         <v>11</v>
       </c>
       <c r="I13" s="20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>187</v>
+        <v>210</v>
       </c>
       <c r="K13" s="21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L13" s="22" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="19" t="s">
-        <v>151</v>
-      </c>
+      <c r="N13" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O13" s="19"/>
       <c r="P13" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q13" s="14" t="s">
-        <v>146</v>
+        <v>20</v>
+      </c>
+      <c r="Q13" s="14">
+        <v>6</v>
       </c>
       <c r="R13" s="15" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="S13" s="14" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="T13" s="16" t="s">
-        <v>186</v>
+        <v>204</v>
       </c>
       <c r="U13" s="14" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2415,31 +2451,31 @@
         <v>155</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F14" s="25"/>
       <c r="G14" s="9" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="H14" s="8">
         <v>12</v>
       </c>
       <c r="I14" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>205</v>
+        <v>172</v>
       </c>
       <c r="K14" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L14" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23" t="s">
-        <v>32</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="M14" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="N14" s="23"/>
       <c r="O14" s="19"/>
       <c r="P14" s="19" t="s">
         <v>19</v>
@@ -2448,19 +2484,19 @@
         <v>6</v>
       </c>
       <c r="R14" s="15" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="S14" s="14" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="T14" s="16" t="s">
-        <v>200</v>
+        <v>173</v>
       </c>
       <c r="U14" s="14" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -2474,11 +2510,11 @@
         <v>155</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F15" s="25"/>
       <c r="G15" s="9" t="s">
-        <v>209</v>
+        <v>168</v>
       </c>
       <c r="H15" s="8">
         <v>13</v>
@@ -2487,36 +2523,34 @@
         <v>20</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>210</v>
+        <v>169</v>
       </c>
       <c r="K15" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L15" s="22" t="s">
         <v>8</v>
       </c>
       <c r="M15" s="23"/>
-      <c r="N15" s="23" t="s">
-        <v>32</v>
-      </c>
+      <c r="N15" s="23"/>
       <c r="O15" s="19"/>
       <c r="P15" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q15" s="14">
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="Q15" s="14" t="s">
+        <v>146</v>
       </c>
       <c r="R15" s="15" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="S15" s="14" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="T15" s="16" t="s">
-        <v>204</v>
+        <v>168</v>
       </c>
       <c r="U15" s="14" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:21" s="50" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4359,25 +4393,25 @@
           <x14:formula1>
             <xm:f>DATOS!$E$14:$E$48</xm:f>
           </x14:formula1>
-          <xm:sqref>N27:N69 N3:N25</xm:sqref>
+          <xm:sqref>N27:N69 N3:N10 N11:N25</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$D$1:$D$2</xm:f>
           </x14:formula1>
-          <xm:sqref>I27:I69 K27:K69 P27:P69 K3:K23 I3:I23 P3:P23</xm:sqref>
+          <xm:sqref>I27:I69 K27:K69 P27:P69 K3:K10 K11:K23 I3:I10 I11:I23 P3:P10 P11:P23</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$B$1:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>L27:L69 L3:L23</xm:sqref>
+          <xm:sqref>L27:L69 L3:L10 L11:L23</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$E$1:$E$13</xm:f>
           </x14:formula1>
-          <xm:sqref>M27:M69 M3:M23</xm:sqref>
+          <xm:sqref>M27:M69 M3:M10 M11:M23</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -4389,7 +4423,7 @@
           <x14:formula1>
             <xm:f>DATOS!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A69</xm:sqref>
+          <xm:sqref>A3:A10 A11:A69</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>